<commit_message>
Acabado Test Case Excel
</commit_message>
<xml_diff>
--- a/M05/ShinyTest Case.xlsx
+++ b/M05/ShinyTest Case.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="156">
   <si>
     <t xml:space="preserve">Project name:</t>
   </si>
@@ -371,6 +371,9 @@
     <t xml:space="preserve">(9) CoNtRaSeñA1</t>
   </si>
   <si>
+    <t xml:space="preserve">Error: not repeated password</t>
+  </si>
+  <si>
     <t xml:space="preserve">(10) Not_another_pass1</t>
   </si>
   <si>
@@ -398,6 +401,9 @@
     <t xml:space="preserve">(14) pablo@localhost</t>
   </si>
   <si>
+    <t xml:space="preserve">Doesn’t fully recognize localhost as valid</t>
+  </si>
+  <si>
     <t xml:space="preserve">(15) www.yahoo.es</t>
   </si>
   <si>
@@ -410,65 +416,49 @@
     <t xml:space="preserve">(17) Bold_one@kamisama.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Error: email already used</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login</t>
   </si>
   <si>
-    <t xml:space="preserve">2- The actor has to click on create alarm button and insert the name of alarm and date.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) Fiestas de bilbao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) Las mejores fiestas del pais vasco
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3) Semana Grand3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4) Bilboko H%iak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error: Name not valid. Is empty.</t>
+    <t xml:space="preserve">1- For login, first introduce username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6) Pete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error: name not found</t>
   </si>
   <si>
     <t xml:space="preserve">Password [valid, invalid]</t>
   </si>
   <si>
-    <t xml:space="preserve">(6) 2013-05-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(7) 18/05/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error: Date not valid. Invalid format.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(8) 03-17-2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(9) 13/10/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(10) 13/12/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(11) 2013-05-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(12) 1999-06-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error: Date on past not valid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error: Date not valid. Is empty.</t>
+    <t xml:space="preserve">2- Then the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7) Kakarot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8) !!!!Paaaac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(9) Bonparapara1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10) CoNtRaSeñA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11) Not_another_pass1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(12) @Flyingfree4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(13) [Whitespace]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error: pass cannot be empty</t>
   </si>
   <si>
     <t xml:space="preserve">Change template</t>
@@ -477,7 +467,31 @@
     <t xml:space="preserve">Select[templates]</t>
   </si>
   <si>
-    <t xml:space="preserve">date [valid, invalid]</t>
+    <t xml:space="preserve">1- User selects a template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Cerulean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Cosmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3) Cyborg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4) Darkly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5) Flatly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6) Journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7) Lumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8) Paper</t>
   </si>
 </sst>
 </file>
@@ -550,16 +564,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -802,52 +817,52 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -923,8 +938,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla5" displayName="Tabla5" ref="A8:I79" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A8:I79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla5" displayName="Tabla5" ref="A8:I72" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A8:I72"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Test Case#"/>
     <tableColumn id="2" name="Test Title"/>
@@ -957,8 +972,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1379,7 +1394,7 @@
       <c r="B23" s="25"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="17" t="s">
         <v>62</v>
       </c>
       <c r="F23" s="17" t="s">
@@ -1456,7 +1471,7 @@
       <c r="G27" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="32"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="20" t="s">
         <v>68</v>
       </c>
@@ -1498,7 +1513,7 @@
       <c r="G29" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="20" t="s">
         <v>77</v>
       </c>
@@ -1513,7 +1528,7 @@
       <c r="C30" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="18" t="s">
@@ -1621,31 +1636,31 @@
       <c r="H35" s="19"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="33" t="s">
+    <row r="36" s="37" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E36" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="34" t="s">
         <v>26</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H36" s="19"/>
-      <c r="I36" s="37"/>
-      <c r="AMJ36" s="39"/>
+      <c r="I36" s="36"/>
+      <c r="AMJ36" s="38"/>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="s">
@@ -1714,7 +1729,7 @@
       <c r="G40" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H40" s="32"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="20" t="s">
         <v>105</v>
       </c>
@@ -1727,7 +1742,7 @@
       <c r="E41" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="34" t="s">
         <v>26</v>
       </c>
       <c r="G41" s="17" t="s">
@@ -1745,7 +1760,7 @@
       <c r="D42" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="39" t="s">
         <v>109</v>
       </c>
       <c r="F42" s="17" t="s">
@@ -1762,7 +1777,7 @@
       <c r="B43" s="25"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="39" t="s">
         <v>111</v>
       </c>
       <c r="F43" s="17" t="s">
@@ -1779,7 +1794,7 @@
       <c r="B44" s="25"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="39" t="s">
         <v>113</v>
       </c>
       <c r="F44" s="17" t="s">
@@ -1800,10 +1815,10 @@
         <v>114</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="20"/>
@@ -1814,7 +1829,7 @@
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>26</v>
@@ -1831,7 +1846,7 @@
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>26</v>
@@ -1839,22 +1854,22 @@
       <c r="G47" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H47" s="41"/>
+      <c r="H47" s="40"/>
       <c r="I47" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="24"/>
       <c r="B48" s="25"/>
       <c r="C48" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F48" s="17" t="s">
         <v>26</v>
@@ -1871,10 +1886,10 @@
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>26</v>
@@ -1888,96 +1903,110 @@
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
       <c r="E50" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H50" s="31"/>
+      <c r="I50" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="24"/>
       <c r="B51" s="25"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
       <c r="E51" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
+        <v>127</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H51" s="19"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="24"/>
       <c r="B52" s="25"/>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
       <c r="E52" s="30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
+      <c r="G52" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" s="19"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="24"/>
       <c r="B53" s="25"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
       <c r="E53" s="30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
+        <v>130</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="19"/>
       <c r="I53" s="20"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="42" t="s">
-        <v>128</v>
+      <c r="B54" s="41" t="s">
+        <v>131</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>93</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="20"/>
-    </row>
-    <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H54" s="19"/>
+      <c r="I54" s="36"/>
+    </row>
+    <row r="55" customFormat="false" ht="17.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="24"/>
       <c r="B55" s="25"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="29" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
+      <c r="G55" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="19"/>
       <c r="I55" s="20"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,13 +2015,15 @@
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
       <c r="E56" s="18" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
+        <v>100</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" s="19"/>
       <c r="I56" s="20"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2001,13 +2032,15 @@
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="18" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="F57" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
+      <c r="G57" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H57" s="19"/>
       <c r="I57" s="20"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,30 +2049,34 @@
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
       <c r="E58" s="18" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="20"/>
+        <v>104</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H58" s="31"/>
+      <c r="I58" s="20" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="24"/>
       <c r="B59" s="25"/>
-      <c r="C59" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="C59" s="17"/>
       <c r="D59" s="17"/>
-      <c r="E59" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
+      <c r="E59" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="19"/>
       <c r="I59" s="20"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,29 +2084,37 @@
       <c r="B60" s="25"/>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
-      <c r="E60" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="F60" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
+      <c r="E60" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" s="19"/>
       <c r="I60" s="20"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="24"/>
       <c r="B61" s="25"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="18" t="s">
-        <v>140</v>
+      <c r="C61" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="39" t="s">
+        <v>137</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
+        <v>110</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="19"/>
       <c r="I61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,14 +2122,16 @@
       <c r="B62" s="25"/>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
-      <c r="E62" s="30" t="s">
-        <v>141</v>
+      <c r="E62" s="39" t="s">
+        <v>138</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
+        <v>112</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="19"/>
       <c r="I62" s="20"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2092,14 +2139,16 @@
       <c r="B63" s="25"/>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
-      <c r="E63" s="30" t="s">
-        <v>142</v>
+      <c r="E63" s="39" t="s">
+        <v>139</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" s="19"/>
       <c r="I63" s="20"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,14 +2156,16 @@
       <c r="B64" s="25"/>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
-      <c r="E64" s="40" t="s">
-        <v>143</v>
+      <c r="E64" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
+        <v>115</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H64" s="19"/>
       <c r="I64" s="20"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,14 +2173,16 @@
       <c r="B65" s="25"/>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
-      <c r="E65" s="40" t="s">
-        <v>144</v>
+      <c r="E65" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="19"/>
       <c r="I65" s="20"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,67 +2190,77 @@
       <c r="B66" s="25"/>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
-      <c r="E66" s="18" t="s">
+      <c r="E66" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H66" s="40"/>
+      <c r="I66" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H67" s="19"/>
+      <c r="I67" s="20"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="F66" s="17" t="s">
+      <c r="D68" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="20"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="42" t="s">
+      <c r="E68" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="20"/>
-    </row>
-    <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="29" t="s">
-        <v>131</v>
-      </c>
       <c r="F68" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H68" s="19"/>
       <c r="I68" s="20"/>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="24"/>
       <c r="B69" s="25"/>
       <c r="C69" s="17"/>
       <c r="D69" s="17"/>
-      <c r="E69" s="18" t="s">
-        <v>132</v>
+      <c r="E69" s="29" t="s">
+        <v>149</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="19"/>
       <c r="I69" s="20"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,13 +2269,15 @@
       <c r="C70" s="17"/>
       <c r="D70" s="17"/>
       <c r="E70" s="18" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H70" s="19"/>
       <c r="I70" s="20"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,137 +2286,104 @@
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
       <c r="E71" s="18" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="19"/>
       <c r="I71" s="20"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="24"/>
       <c r="B72" s="25"/>
-      <c r="C72" s="17" t="s">
-        <v>150</v>
-      </c>
+      <c r="C72" s="17"/>
       <c r="D72" s="17"/>
-      <c r="E72" s="40" t="s">
-        <v>137</v>
+      <c r="E72" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="F72" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
+      <c r="G72" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" s="19"/>
       <c r="I72" s="20"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="24"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="30" t="s">
-        <v>138</v>
+      <c r="E73" s="42" t="s">
+        <v>153</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="19"/>
+      <c r="I73" s="42"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="24"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="18" t="s">
-        <v>140</v>
+      <c r="E74" s="42" t="s">
+        <v>154</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H74" s="19"/>
+      <c r="I74" s="42"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="24"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="30" t="s">
-        <v>141</v>
+      <c r="E75" s="42" t="s">
+        <v>155</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" s="19"/>
+      <c r="I75" s="42"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="20"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="24"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="20"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="42"/>
+      <c r="H77" s="42"/>
+      <c r="I77" s="42"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="24"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="20"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="42"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="24"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="20"/>
-    </row>
+      <c r="F79" s="42"/>
+      <c r="G79" s="42"/>
+      <c r="H79" s="42"/>
+      <c r="I79" s="42"/>
+    </row>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2463,11 +2495,11 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E48" r:id="rId1" display="comolagente44@hotmail.com"/>
-    <hyperlink ref="E50" r:id="rId2" display="pablo@localhost"/>
-    <hyperlink ref="E51" r:id="rId3" display="www.yahoo.es"/>
-    <hyperlink ref="E52" r:id="rId4" display="User@yahoo.es"/>
-    <hyperlink ref="E53" r:id="rId5" display="Bold_one@kamisama.com"/>
+    <hyperlink ref="E48" r:id="rId1" display="(12) comolagente44@hotmail.com"/>
+    <hyperlink ref="E50" r:id="rId2" display="(14) pablo@localhost"/>
+    <hyperlink ref="E51" r:id="rId3" display="(15) www.yahoo.es"/>
+    <hyperlink ref="E52" r:id="rId4" display="(16) User@yahoo.es"/>
+    <hyperlink ref="E53" r:id="rId5" display="(17) Bold_one@kamisama.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>